<commit_message>
only select one newest record for excel update
</commit_message>
<xml_diff>
--- a/data/name/en.given.v1.xlsx
+++ b/data/name/en.given.v1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D589501D-E9C9-9F49-B76B-C8AA25A33B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CDCC7A-5FB7-5A47-A1FB-FA96057A3C42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="1520" windowWidth="20940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6166,7 +6166,7 @@
   <dimension ref="A1:D2001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14"/>

</xml_diff>